<commit_message>
Update MasterCodebook_Final_June2022 ALL (Repaired).xlsx
</commit_message>
<xml_diff>
--- a/1_Input_data/MasterCodebook_Final_June2022 ALL (Repaired).xlsx
+++ b/1_Input_data/MasterCodebook_Final_June2022 ALL (Repaired).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdamen/Documents/GitHub/Zika_imputation/1_Input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFF9128-E21C-194E-8010-2A0B9631DAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C9EC89-8183-C54F-9BA7-581F3C875EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{EB9D8945-92F8-48A6-B1A8-0874D0F705AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -670,7 +670,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12266" uniqueCount="2896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12269" uniqueCount="2897">
   <si>
     <t>Tab</t>
   </si>
@@ -11140,6 +11140,9 @@
   </si>
   <si>
     <t>comorbid_preg</t>
+  </si>
+  <si>
+    <t>drug_tera</t>
   </si>
 </sst>
 </file>
@@ -11808,7 +11811,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12451,16 +12454,19 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -47787,14 +47793,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B522DC56-3FF5-3344-845C-95A0430599ED}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:S249"/>
+  <dimension ref="A1:S250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B199" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M244" sqref="M244"/>
+      <selection pane="bottomRight" activeCell="E220" sqref="E220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -47870,7 +47875,7 @@
         <v>2845</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" s="177" t="s">
         <v>123</v>
       </c>
@@ -47907,7 +47912,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="177" t="s">
         <v>128</v>
       </c>
@@ -47944,7 +47949,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" s="177" t="s">
         <v>132</v>
       </c>
@@ -47981,7 +47986,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="5" spans="1:19" ht="15" customHeight="1">
       <c r="A5" s="177" t="s">
         <v>136</v>
       </c>
@@ -48015,7 +48020,7 @@
         <v>76.291901936959505</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="6" spans="1:19" ht="15" customHeight="1">
       <c r="A6" s="177" t="s">
         <v>138</v>
       </c>
@@ -48049,7 +48054,7 @@
         <v>77.342577371167195</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="7" spans="1:19" ht="15" customHeight="1">
       <c r="A7" s="177" t="s">
         <v>140</v>
       </c>
@@ -48084,7 +48089,7 @@
       </c>
       <c r="N7" s="223"/>
     </row>
-    <row r="8" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="8" spans="1:19" ht="15" customHeight="1">
       <c r="A8" s="177" t="s">
         <v>142</v>
       </c>
@@ -48119,7 +48124,7 @@
       </c>
       <c r="N8" s="223"/>
     </row>
-    <row r="9" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="9" spans="1:19" ht="15" customHeight="1">
       <c r="A9" s="177" t="s">
         <v>144</v>
       </c>
@@ -48154,7 +48159,7 @@
       </c>
       <c r="N9" s="223"/>
     </row>
-    <row r="10" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="10" spans="1:19" ht="15" customHeight="1">
       <c r="A10" s="177" t="s">
         <v>146</v>
       </c>
@@ -48380,7 +48385,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="15" spans="1:19" ht="15" customHeight="1">
       <c r="A15" s="177" t="s">
         <v>180</v>
       </c>
@@ -48468,7 +48473,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="17" spans="1:18" ht="15" customHeight="1">
       <c r="A17" s="177" t="s">
         <v>208</v>
       </c>
@@ -48506,7 +48511,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="18" spans="1:18" ht="15" customHeight="1">
       <c r="A18" s="177" t="s">
         <v>247</v>
       </c>
@@ -48544,7 +48549,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="19" spans="1:18" ht="15" customHeight="1">
       <c r="A19" s="177" t="s">
         <v>250</v>
       </c>
@@ -48582,7 +48587,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="20" spans="1:18" ht="15" customHeight="1">
       <c r="A20" s="177" t="s">
         <v>254</v>
       </c>
@@ -48665,7 +48670,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="22" spans="1:18" ht="15" customHeight="1">
       <c r="A22" s="214" t="s">
         <v>269</v>
       </c>
@@ -48708,7 +48713,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="23" spans="1:18" ht="15" customHeight="1">
       <c r="A23" s="193" t="s">
         <v>309</v>
       </c>
@@ -48751,7 +48756,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="24" spans="1:18" ht="15" customHeight="1">
       <c r="A24" s="177" t="s">
         <v>332</v>
       </c>
@@ -48794,7 +48799,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="25" spans="1:18" ht="15" customHeight="1">
       <c r="A25" s="177" t="s">
         <v>347</v>
       </c>
@@ -48837,7 +48842,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="26" spans="1:18" ht="15" customHeight="1">
       <c r="A26" s="177" t="s">
         <v>361</v>
       </c>
@@ -48880,7 +48885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="27" spans="1:18" ht="15" customHeight="1">
       <c r="A27" s="193" t="s">
         <v>365</v>
       </c>
@@ -48923,7 +48928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="28" spans="1:18" ht="15" customHeight="1">
       <c r="A28" s="193" t="s">
         <v>369</v>
       </c>
@@ -48961,7 +48966,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="29" spans="1:18" ht="15" customHeight="1">
       <c r="A29" s="215" t="s">
         <v>372</v>
       </c>
@@ -48999,7 +49004,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="30" spans="1:18" ht="15" customHeight="1">
       <c r="A30" s="215" t="s">
         <v>374</v>
       </c>
@@ -49038,7 +49043,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="31" spans="1:18" ht="15" customHeight="1">
       <c r="A31" s="215" t="s">
         <v>376</v>
       </c>
@@ -49077,7 +49082,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="32" spans="1:18" ht="15" customHeight="1">
       <c r="A32" s="215" t="s">
         <v>378</v>
       </c>
@@ -49115,7 +49120,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="33" spans="1:16" ht="15" customHeight="1">
       <c r="A33" s="193" t="s">
         <v>380</v>
       </c>
@@ -49152,7 +49157,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="34" spans="1:16" ht="15" customHeight="1">
       <c r="A34" s="193" t="s">
         <v>382</v>
       </c>
@@ -49191,7 +49196,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="35" spans="1:16" ht="15" customHeight="1">
       <c r="A35" s="193" t="s">
         <v>385</v>
       </c>
@@ -49228,7 +49233,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="36" spans="1:16" ht="15" customHeight="1">
       <c r="A36" s="216" t="s">
         <v>395</v>
       </c>
@@ -49271,7 +49276,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="37" spans="1:16" ht="15" customHeight="1">
       <c r="A37" s="177" t="s">
         <v>397</v>
       </c>
@@ -49314,7 +49319,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="38" spans="1:16" ht="15" customHeight="1">
       <c r="A38" s="215" t="s">
         <v>400</v>
       </c>
@@ -49354,7 +49359,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="39" spans="1:16" ht="15" customHeight="1">
       <c r="A39" s="193" t="s">
         <v>403</v>
       </c>
@@ -49391,7 +49396,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="40" spans="1:16" ht="15" customHeight="1">
       <c r="A40" s="193" t="s">
         <v>405</v>
       </c>
@@ -49428,7 +49433,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="41" spans="1:16" ht="15" customHeight="1">
       <c r="A41" s="193" t="s">
         <v>408</v>
       </c>
@@ -49460,7 +49465,7 @@
         <v>98.499035093988994</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="42" spans="1:16" ht="15" customHeight="1">
       <c r="A42" s="177" t="s">
         <v>414</v>
       </c>
@@ -49503,7 +49508,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="43" spans="1:16" ht="15" customHeight="1">
       <c r="A43" s="193" t="s">
         <v>416</v>
       </c>
@@ -49548,7 +49553,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="44" spans="1:16" ht="15" customHeight="1">
       <c r="A44" s="177" t="s">
         <v>437</v>
       </c>
@@ -49591,7 +49596,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="45" spans="1:16" ht="15" customHeight="1">
       <c r="A45" s="177" t="s">
         <v>439</v>
       </c>
@@ -49634,7 +49639,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="46" spans="1:16" ht="15" customHeight="1">
       <c r="A46" s="177" t="s">
         <v>441</v>
       </c>
@@ -49677,7 +49682,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="47" spans="1:16" ht="15" customHeight="1">
       <c r="A47" s="193" t="s">
         <v>454</v>
       </c>
@@ -49720,7 +49725,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="48" spans="1:16" ht="15" customHeight="1">
       <c r="A48" s="193" t="s">
         <v>457</v>
       </c>
@@ -49757,7 +49762,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="49" spans="1:19" ht="15" customHeight="1">
       <c r="A49" s="177" t="s">
         <v>2648</v>
       </c>
@@ -49805,7 +49810,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="50" spans="1:19" ht="15" customHeight="1">
       <c r="A50" s="193" t="s">
         <v>465</v>
       </c>
@@ -49859,7 +49864,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="51" spans="1:19" ht="15" customHeight="1">
       <c r="A51" s="177" t="s">
         <v>467</v>
       </c>
@@ -49913,7 +49918,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="52" spans="1:19" ht="15" customHeight="1">
       <c r="A52" s="193" t="s">
         <v>469</v>
       </c>
@@ -49958,7 +49963,7 @@
         <v>2875</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="53" spans="1:19" ht="15" customHeight="1">
       <c r="A53" s="193" t="s">
         <v>472</v>
       </c>
@@ -50001,7 +50006,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="54" spans="1:19" ht="15" customHeight="1">
       <c r="A54" s="215" t="s">
         <v>474</v>
       </c>
@@ -50046,7 +50051,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="55" spans="1:19" ht="15" customHeight="1">
       <c r="A55" s="215" t="s">
         <v>478</v>
       </c>
@@ -50085,7 +50090,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="56" spans="1:19" ht="15" customHeight="1">
       <c r="A56" s="177" t="s">
         <v>482</v>
       </c>
@@ -50125,7 +50130,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="57" spans="1:19" ht="15" customHeight="1">
       <c r="A57" s="215" t="s">
         <v>484</v>
       </c>
@@ -50176,7 +50181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="58" spans="1:19" ht="15" customHeight="1">
       <c r="A58" s="177" t="s">
         <v>488</v>
       </c>
@@ -50219,7 +50224,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="59" spans="1:19" ht="15" customHeight="1">
       <c r="A59" s="217" t="s">
         <v>490</v>
       </c>
@@ -50264,7 +50269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="60" spans="1:19" ht="15" customHeight="1">
       <c r="A60" s="215" t="s">
         <v>493</v>
       </c>
@@ -50307,7 +50312,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="61" spans="1:19" ht="15" customHeight="1">
       <c r="A61" s="177" t="s">
         <v>495</v>
       </c>
@@ -50350,7 +50355,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="62" spans="1:19" ht="15" customHeight="1">
       <c r="A62" s="177" t="s">
         <v>497</v>
       </c>
@@ -50440,7 +50445,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="64" spans="1:19" ht="15" customHeight="1">
       <c r="A64" s="215" t="s">
         <v>530</v>
       </c>
@@ -50483,7 +50488,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="65" spans="1:16" ht="15" customHeight="1">
       <c r="A65" s="193" t="s">
         <v>533</v>
       </c>
@@ -50526,7 +50531,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="66" spans="1:16" ht="15" customHeight="1">
       <c r="A66" s="215" t="s">
         <v>535</v>
       </c>
@@ -50569,7 +50574,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="67" spans="1:16" ht="15" customHeight="1">
       <c r="A67" s="215" t="s">
         <v>537</v>
       </c>
@@ -50612,7 +50617,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="68" spans="1:16" ht="15" customHeight="1">
       <c r="A68" s="215" t="s">
         <v>539</v>
       </c>
@@ -50655,7 +50660,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="69" spans="1:16" ht="15" customHeight="1">
       <c r="A69" s="215" t="s">
         <v>542</v>
       </c>
@@ -50692,7 +50697,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="70" spans="1:16" ht="15" customHeight="1">
       <c r="A70" s="215" t="s">
         <v>544</v>
       </c>
@@ -50735,7 +50740,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="71" spans="1:16" ht="15" customHeight="1">
       <c r="A71" s="215" t="s">
         <v>546</v>
       </c>
@@ -50778,7 +50783,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="72" spans="1:16" ht="15" customHeight="1">
       <c r="A72" s="215" t="s">
         <v>548</v>
       </c>
@@ -50821,7 +50826,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="73" spans="1:16" ht="15" customHeight="1">
       <c r="A73" s="177" t="s">
         <v>550</v>
       </c>
@@ -50864,7 +50869,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="74" spans="1:16" ht="15" customHeight="1">
       <c r="A74" s="177" t="s">
         <v>552</v>
       </c>
@@ -50907,7 +50912,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="75" spans="1:16" ht="15" customHeight="1">
       <c r="A75" s="215" t="s">
         <v>554</v>
       </c>
@@ -50950,7 +50955,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="76" spans="1:16" ht="15" customHeight="1">
       <c r="A76" s="215" t="s">
         <v>556</v>
       </c>
@@ -50993,7 +50998,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="77" spans="1:16" ht="15" customHeight="1">
       <c r="A77" s="215" t="s">
         <v>558</v>
       </c>
@@ -51036,7 +51041,7 @@
         <v>2872</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="78" spans="1:16" ht="15" customHeight="1">
       <c r="A78" s="215" t="s">
         <v>560</v>
       </c>
@@ -51259,7 +51264,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="83" spans="1:19" ht="15" customHeight="1">
       <c r="A83" s="177" t="s">
         <v>704</v>
       </c>
@@ -51302,7 +51307,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="84" spans="1:19" ht="15" customHeight="1">
       <c r="A84" s="177" t="s">
         <v>710</v>
       </c>
@@ -51339,7 +51344,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="85" spans="1:19" ht="15" customHeight="1">
       <c r="A85" s="177" t="s">
         <v>712</v>
       </c>
@@ -51391,7 +51396,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="86" spans="1:19" ht="15" customHeight="1">
       <c r="A86" s="177" t="s">
         <v>715</v>
       </c>
@@ -51434,7 +51439,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="87" spans="1:19" ht="15" customHeight="1">
       <c r="A87" s="177" t="s">
         <v>717</v>
       </c>
@@ -51479,7 +51484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="88" spans="1:19" ht="15" customHeight="1">
       <c r="A88" s="177" t="s">
         <v>721</v>
       </c>
@@ -51569,7 +51574,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="90" spans="1:19" ht="15" customHeight="1">
       <c r="A90" s="177" t="s">
         <v>728</v>
       </c>
@@ -51618,7 +51623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="91" spans="1:19" ht="15" customHeight="1">
       <c r="A91" s="193" t="s">
         <v>733</v>
       </c>
@@ -51657,7 +51662,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="92" spans="1:19" ht="15" customHeight="1">
       <c r="A92" s="177" t="s">
         <v>739</v>
       </c>
@@ -51753,7 +51758,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="94" spans="1:19" ht="15" customHeight="1">
       <c r="A94" s="177" t="s">
         <v>744</v>
       </c>
@@ -51802,7 +51807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="95" spans="1:19" ht="15" customHeight="1">
       <c r="A95" s="177" t="s">
         <v>746</v>
       </c>
@@ -51853,7 +51858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="96" spans="1:19" ht="15" customHeight="1">
       <c r="A96" s="177" t="s">
         <v>748</v>
       </c>
@@ -51943,7 +51948,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="98" spans="1:19" ht="15" customHeight="1">
       <c r="A98" s="177" t="s">
         <v>753</v>
       </c>
@@ -52037,7 +52042,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="100" spans="1:19" ht="15" customHeight="1">
       <c r="A100" s="177" t="s">
         <v>757</v>
       </c>
@@ -52403,7 +52408,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="108" spans="1:19" ht="15" customHeight="1">
       <c r="A108" s="194" t="s">
         <v>791</v>
       </c>
@@ -52446,7 +52451,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="109" spans="1:19" ht="15" customHeight="1">
       <c r="A109" s="194" t="s">
         <v>798</v>
       </c>
@@ -52489,7 +52494,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="110" spans="1:19" ht="15" customHeight="1">
       <c r="A110" s="194" t="s">
         <v>802</v>
       </c>
@@ -52538,7 +52543,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="111" spans="1:19" ht="15" customHeight="1">
       <c r="A111" s="194" t="s">
         <v>805</v>
       </c>
@@ -52578,7 +52583,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="112" spans="1:19" ht="15" customHeight="1">
       <c r="A112" s="194" t="s">
         <v>809</v>
       </c>
@@ -52620,7 +52625,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="113" spans="1:19" ht="15" customHeight="1">
       <c r="A113" s="194" t="s">
         <v>811</v>
       </c>
@@ -52674,7 +52679,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="114" spans="1:19" ht="15" customHeight="1">
       <c r="A114" s="194" t="s">
         <v>813</v>
       </c>
@@ -52719,7 +52724,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="115" spans="1:19" ht="15" customHeight="1">
       <c r="A115" s="194" t="s">
         <v>815</v>
       </c>
@@ -52761,7 +52766,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="116" spans="1:19" ht="15" customHeight="1">
       <c r="A116" s="194" t="s">
         <v>829</v>
       </c>
@@ -52815,7 +52820,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="117" spans="1:19" ht="15" customHeight="1">
       <c r="A117" s="194" t="s">
         <v>832</v>
       </c>
@@ -52857,7 +52862,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="118" spans="1:19" ht="15" customHeight="1">
       <c r="A118" s="194" t="s">
         <v>835</v>
       </c>
@@ -52952,7 +52957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="120" spans="1:19" ht="15" customHeight="1">
       <c r="A120" s="194" t="s">
         <v>842</v>
       </c>
@@ -52991,7 +52996,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="121" spans="1:19" ht="15" customHeight="1">
       <c r="A121" s="194" t="s">
         <v>846</v>
       </c>
@@ -53033,7 +53038,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="122" spans="1:19" ht="15" customHeight="1">
       <c r="A122" s="194" t="s">
         <v>850</v>
       </c>
@@ -53087,7 +53092,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="123" spans="1:19" ht="15" customHeight="1">
       <c r="A123" s="194" t="s">
         <v>852</v>
       </c>
@@ -53129,7 +53134,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="124" spans="1:19" ht="15" customHeight="1">
       <c r="A124" s="194" t="s">
         <v>854</v>
       </c>
@@ -53171,7 +53176,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="125" spans="1:19" ht="15" customHeight="1">
       <c r="A125" s="194" t="s">
         <v>856</v>
       </c>
@@ -53213,7 +53218,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="126" spans="1:19" ht="15" customHeight="1">
       <c r="A126" s="194" t="s">
         <v>860</v>
       </c>
@@ -53255,7 +53260,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="127" spans="1:19" ht="15" customHeight="1">
       <c r="A127" s="194" t="s">
         <v>864</v>
       </c>
@@ -53297,7 +53302,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="128" spans="1:19" ht="15" customHeight="1">
       <c r="A128" s="194" t="s">
         <v>870</v>
       </c>
@@ -53339,7 +53344,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="129" spans="1:19" ht="15" customHeight="1">
       <c r="A129" s="194" t="s">
         <v>874</v>
       </c>
@@ -53387,7 +53392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="130" spans="1:19" ht="15" customHeight="1">
       <c r="A130" s="194" t="s">
         <v>879</v>
       </c>
@@ -53429,7 +53434,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="131" spans="1:19" ht="15" customHeight="1">
       <c r="A131" s="194" t="s">
         <v>881</v>
       </c>
@@ -53477,7 +53482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="132" spans="1:19" ht="15" customHeight="1">
       <c r="A132" s="194" t="s">
         <v>885</v>
       </c>
@@ -53525,7 +53530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="133" spans="1:19" ht="15" customHeight="1">
       <c r="A133" s="194" t="s">
         <v>890</v>
       </c>
@@ -53567,7 +53572,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="134" spans="1:19" ht="15" customHeight="1">
       <c r="A134" s="194" t="s">
         <v>894</v>
       </c>
@@ -53618,7 +53623,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="135" spans="1:19" ht="15" customHeight="1">
       <c r="A135" s="194" t="s">
         <v>898</v>
       </c>
@@ -53666,7 +53671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="136" spans="1:19" ht="15" customHeight="1">
       <c r="A136" s="194" t="s">
         <v>901</v>
       </c>
@@ -53714,7 +53719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="137" spans="1:19" ht="15" customHeight="1">
       <c r="A137" s="194" t="s">
         <v>905</v>
       </c>
@@ -53759,7 +53764,7 @@
         <v>2856</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="138" spans="1:19" ht="15" customHeight="1">
       <c r="A138" s="194" t="s">
         <v>909</v>
       </c>
@@ -53858,7 +53863,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="140" spans="1:19" ht="15" customHeight="1">
       <c r="A140" s="194" t="s">
         <v>916</v>
       </c>
@@ -53948,7 +53953,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="142" spans="1:19" ht="15" customHeight="1">
       <c r="A142" s="194" t="s">
         <v>921</v>
       </c>
@@ -53988,7 +53993,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="143" spans="1:19" ht="15" customHeight="1">
       <c r="A143" s="194" t="s">
         <v>924</v>
       </c>
@@ -54031,7 +54036,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="144" spans="1:19" ht="15" customHeight="1">
       <c r="A144" s="194" t="s">
         <v>931</v>
       </c>
@@ -54070,7 +54075,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="145" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="145" spans="1:18" ht="15" customHeight="1">
       <c r="A145" s="194" t="s">
         <v>934</v>
       </c>
@@ -54118,7 +54123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="146" spans="1:18" ht="15" customHeight="1">
       <c r="A146" s="194" t="s">
         <v>938</v>
       </c>
@@ -54157,7 +54162,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="147" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="147" spans="1:18" ht="15" customHeight="1">
       <c r="A147" s="194" t="s">
         <v>941</v>
       </c>
@@ -54205,7 +54210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="148" spans="1:18" ht="15" customHeight="1">
       <c r="A148" s="194" t="s">
         <v>945</v>
       </c>
@@ -54244,7 +54249,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="149" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="149" spans="1:18" ht="15" customHeight="1">
       <c r="A149" s="194" t="s">
         <v>947</v>
       </c>
@@ -54292,7 +54297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="150" spans="1:18" ht="15" customHeight="1">
       <c r="A150" s="194" t="s">
         <v>949</v>
       </c>
@@ -54340,7 +54345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="151" spans="1:18" ht="15" customHeight="1">
       <c r="A151" s="194" t="s">
         <v>960</v>
       </c>
@@ -54383,7 +54388,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="152" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="152" spans="1:18" ht="15" customHeight="1">
       <c r="A152" s="194" t="s">
         <v>966</v>
       </c>
@@ -54422,7 +54427,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="153" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="153" spans="1:18" ht="15" customHeight="1">
       <c r="A153" s="194" t="s">
         <v>969</v>
       </c>
@@ -54470,7 +54475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="154" spans="1:18" ht="15" customHeight="1">
       <c r="A154" s="194" t="s">
         <v>973</v>
       </c>
@@ -54509,7 +54514,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="155" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="155" spans="1:18" ht="15" customHeight="1">
       <c r="A155" s="194" t="s">
         <v>976</v>
       </c>
@@ -54557,7 +54562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="156" spans="1:18" ht="15" customHeight="1">
       <c r="A156" s="194" t="s">
         <v>980</v>
       </c>
@@ -54596,7 +54601,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="157" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="157" spans="1:18" ht="15" customHeight="1">
       <c r="A157" s="194" t="s">
         <v>983</v>
       </c>
@@ -54644,7 +54649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="158" spans="1:18" ht="15" customHeight="1">
       <c r="A158" s="207" t="s">
         <v>1663</v>
       </c>
@@ -54678,7 +54683,7 @@
         <v>13.4086198270317</v>
       </c>
     </row>
-    <row r="159" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="159" spans="1:18" ht="15" customHeight="1">
       <c r="A159" s="207" t="s">
         <v>1660</v>
       </c>
@@ -54715,7 +54720,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="160" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="160" spans="1:18" ht="15" customHeight="1">
       <c r="A160" s="207" t="s">
         <v>1658</v>
       </c>
@@ -54804,7 +54809,7 @@
         <v>120</v>
       </c>
       <c r="D162" s="218"/>
-      <c r="E162" s="238" t="s">
+      <c r="E162" s="237" t="s">
         <v>120</v>
       </c>
       <c r="F162" s="177">
@@ -54839,7 +54844,7 @@
       </c>
       <c r="P162" s="223"/>
     </row>
-    <row r="163" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="163" spans="1:19" ht="15" customHeight="1">
       <c r="A163" s="203" t="s">
         <v>1042</v>
       </c>
@@ -54877,7 +54882,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="164" spans="1:19" ht="15" customHeight="1">
       <c r="A164" s="203" t="s">
         <v>1039</v>
       </c>
@@ -54924,7 +54929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="165" spans="1:19" ht="15" customHeight="1">
       <c r="A165" s="207" t="s">
         <v>1632</v>
       </c>
@@ -54956,7 +54961,7 @@
         <v>99.749839182331499</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="166" spans="1:19" ht="15" customHeight="1">
       <c r="A166" s="207" t="s">
         <v>1628</v>
       </c>
@@ -54988,7 +54993,7 @@
         <v>99.635479951397301</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="167" spans="1:19" ht="15" customHeight="1">
       <c r="A167" s="207" t="s">
         <v>1625</v>
       </c>
@@ -55022,7 +55027,7 @@
         <v>97.920091487384795</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="168" spans="1:19" ht="15" customHeight="1">
       <c r="A168" s="207" t="s">
         <v>1621</v>
       </c>
@@ -55054,7 +55059,7 @@
         <v>98.827817882924705</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="169" spans="1:19" ht="15" customHeight="1">
       <c r="A169" s="207" t="s">
         <v>1619</v>
       </c>
@@ -55086,7 +55091,7 @@
         <v>99.849903509398899</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="170" spans="1:19" ht="15" customHeight="1">
       <c r="A170" s="207" t="s">
         <v>1616</v>
       </c>
@@ -55118,7 +55123,7 @@
         <v>99.978557644199896</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="171" spans="1:19" ht="15" customHeight="1">
       <c r="A171" s="207" t="s">
         <v>1612</v>
       </c>
@@ -55156,7 +55161,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="172" spans="1:19" ht="15" customHeight="1">
       <c r="A172" s="203" t="s">
         <v>1522</v>
       </c>
@@ -55197,7 +55202,7 @@
       </c>
       <c r="P172" s="223"/>
     </row>
-    <row r="173" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="173" spans="1:19" ht="15" customHeight="1">
       <c r="A173" s="219" t="s">
         <v>1517</v>
       </c>
@@ -55241,7 +55246,7 @@
       </c>
       <c r="P173" s="223"/>
     </row>
-    <row r="174" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="174" spans="1:19" ht="15" customHeight="1">
       <c r="A174" s="207" t="s">
         <v>1511</v>
       </c>
@@ -55282,7 +55287,7 @@
       </c>
       <c r="P174" s="223"/>
     </row>
-    <row r="175" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="175" spans="1:19" ht="15" customHeight="1">
       <c r="A175" s="219" t="s">
         <v>1508</v>
       </c>
@@ -55326,7 +55331,7 @@
       </c>
       <c r="P175" s="223"/>
     </row>
-    <row r="176" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="176" spans="1:19" ht="15" customHeight="1">
       <c r="A176" s="219" t="s">
         <v>1504</v>
       </c>
@@ -55370,7 +55375,7 @@
       </c>
       <c r="P176" s="223"/>
     </row>
-    <row r="177" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="177" spans="1:16" ht="15" customHeight="1">
       <c r="A177" s="219" t="s">
         <v>1490</v>
       </c>
@@ -55414,7 +55419,7 @@
       </c>
       <c r="P177" s="223"/>
     </row>
-    <row r="178" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="178" spans="1:16" ht="15" customHeight="1">
       <c r="A178" s="219" t="s">
         <v>1475</v>
       </c>
@@ -55458,7 +55463,7 @@
       </c>
       <c r="P178" s="223"/>
     </row>
-    <row r="179" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="179" spans="1:16" ht="15" customHeight="1">
       <c r="A179" s="219" t="s">
         <v>1459</v>
       </c>
@@ -55502,7 +55507,7 @@
       </c>
       <c r="P179" s="223"/>
     </row>
-    <row r="180" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="180" spans="1:16" ht="15" customHeight="1">
       <c r="A180" s="219" t="s">
         <v>1445</v>
       </c>
@@ -55546,7 +55551,7 @@
       </c>
       <c r="P180" s="223"/>
     </row>
-    <row r="181" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="181" spans="1:16" ht="15" customHeight="1">
       <c r="A181" s="219" t="s">
         <v>1441</v>
       </c>
@@ -55590,7 +55595,7 @@
       </c>
       <c r="P181" s="223"/>
     </row>
-    <row r="182" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="182" spans="1:16" ht="15" customHeight="1">
       <c r="A182" s="219" t="s">
         <v>1429</v>
       </c>
@@ -55634,7 +55639,7 @@
       </c>
       <c r="P182" s="223"/>
     </row>
-    <row r="183" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="183" spans="1:16" ht="15" customHeight="1">
       <c r="A183" s="207" t="s">
         <v>1419</v>
       </c>
@@ -55675,7 +55680,7 @@
       </c>
       <c r="P183" s="223"/>
     </row>
-    <row r="184" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="184" spans="1:16" ht="15" customHeight="1">
       <c r="A184" s="219" t="s">
         <v>1416</v>
       </c>
@@ -55719,7 +55724,7 @@
       </c>
       <c r="P184" s="223"/>
     </row>
-    <row r="185" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="185" spans="1:16" ht="15" customHeight="1">
       <c r="A185" s="219" t="s">
         <v>1412</v>
       </c>
@@ -55763,7 +55768,7 @@
       </c>
       <c r="P185" s="223"/>
     </row>
-    <row r="186" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="186" spans="1:16" ht="15" customHeight="1">
       <c r="A186" s="219" t="s">
         <v>1396</v>
       </c>
@@ -55807,7 +55812,7 @@
       </c>
       <c r="P186" s="223"/>
     </row>
-    <row r="187" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="187" spans="1:16" ht="15" customHeight="1">
       <c r="A187" s="219" t="s">
         <v>1380</v>
       </c>
@@ -55851,7 +55856,7 @@
       </c>
       <c r="P187" s="223"/>
     </row>
-    <row r="188" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="188" spans="1:16" ht="15" customHeight="1">
       <c r="A188" s="219" t="s">
         <v>1362</v>
       </c>
@@ -55895,7 +55900,7 @@
       </c>
       <c r="P188" s="223"/>
     </row>
-    <row r="189" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="189" spans="1:16" ht="15" customHeight="1">
       <c r="A189" s="219" t="s">
         <v>1345</v>
       </c>
@@ -55939,7 +55944,7 @@
       </c>
       <c r="P189" s="223"/>
     </row>
-    <row r="190" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="190" spans="1:16" ht="15" customHeight="1">
       <c r="A190" s="219" t="s">
         <v>1335</v>
       </c>
@@ -55983,7 +55988,7 @@
       </c>
       <c r="P190" s="223"/>
     </row>
-    <row r="191" spans="1:16" ht="15" hidden="1" customHeight="1">
+    <row r="191" spans="1:16" ht="15" customHeight="1">
       <c r="A191" s="219" t="s">
         <v>1320</v>
       </c>
@@ -56071,7 +56076,7 @@
       </c>
       <c r="P192" s="223"/>
     </row>
-    <row r="193" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="193" spans="1:19" ht="15" customHeight="1">
       <c r="A193" s="203" t="s">
         <v>1189</v>
       </c>
@@ -56115,7 +56120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="194" spans="1:19" ht="15" customHeight="1">
       <c r="A194" s="203" t="s">
         <v>1186</v>
       </c>
@@ -56150,7 +56155,7 @@
       <c r="O194" s="223"/>
       <c r="P194" s="223"/>
     </row>
-    <row r="195" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="195" spans="1:19" ht="15" customHeight="1">
       <c r="A195" s="203" t="s">
         <v>1183</v>
       </c>
@@ -56190,7 +56195,7 @@
       <c r="O195" s="223"/>
       <c r="P195" s="223"/>
     </row>
-    <row r="196" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="196" spans="1:19" ht="15" customHeight="1">
       <c r="A196" s="203" t="s">
         <v>1181</v>
       </c>
@@ -56239,7 +56244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="197" spans="1:19" ht="15" customHeight="1">
       <c r="A197" s="203" t="s">
         <v>1178</v>
       </c>
@@ -56279,7 +56284,7 @@
       <c r="O197" s="223"/>
       <c r="P197" s="223"/>
     </row>
-    <row r="198" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="198" spans="1:19" ht="15" customHeight="1">
       <c r="A198" s="203" t="s">
         <v>1176</v>
       </c>
@@ -56328,7 +56333,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="199" spans="1:19" ht="15" customHeight="1">
       <c r="A199" s="207" t="s">
         <v>1174</v>
       </c>
@@ -56370,7 +56375,7 @@
       <c r="O199" s="223"/>
       <c r="P199" s="223"/>
     </row>
-    <row r="200" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="200" spans="1:19" ht="15" customHeight="1">
       <c r="A200" s="207" t="s">
         <v>1171</v>
       </c>
@@ -56412,7 +56417,7 @@
       <c r="O200" s="223"/>
       <c r="P200" s="223"/>
     </row>
-    <row r="201" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="201" spans="1:19" ht="15" customHeight="1">
       <c r="A201" s="207" t="s">
         <v>1165</v>
       </c>
@@ -56461,7 +56466,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="202" spans="1:19" ht="15" customHeight="1">
       <c r="A202" s="207" t="s">
         <v>1666</v>
       </c>
@@ -56497,7 +56502,7 @@
       <c r="O202" s="223"/>
       <c r="P202" s="223"/>
     </row>
-    <row r="203" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="203" spans="1:19" ht="15" customHeight="1">
       <c r="A203" s="207" t="s">
         <v>1669</v>
       </c>
@@ -56535,7 +56540,7 @@
         <v>2874</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="204" spans="1:19" ht="15" customHeight="1">
       <c r="A204" s="207" t="s">
         <v>1671</v>
       </c>
@@ -56571,7 +56576,7 @@
       <c r="O204" s="223"/>
       <c r="P204" s="223"/>
     </row>
-    <row r="205" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="205" spans="1:19" ht="15" customHeight="1">
       <c r="A205" s="207" t="s">
         <v>1674</v>
       </c>
@@ -56607,7 +56612,7 @@
       <c r="O205" s="223"/>
       <c r="P205" s="223"/>
     </row>
-    <row r="206" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="206" spans="1:19" ht="15" customHeight="1">
       <c r="A206" s="207" t="s">
         <v>1675</v>
       </c>
@@ -56643,7 +56648,7 @@
       <c r="O206" s="223"/>
       <c r="P206" s="223"/>
     </row>
-    <row r="207" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="207" spans="1:19" ht="15" customHeight="1">
       <c r="A207" s="207" t="s">
         <v>1676</v>
       </c>
@@ -56679,7 +56684,7 @@
       <c r="O207" s="223"/>
       <c r="P207" s="223"/>
     </row>
-    <row r="208" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="208" spans="1:19" ht="15" customHeight="1">
       <c r="A208" s="207" t="s">
         <v>1677</v>
       </c>
@@ -56715,7 +56720,7 @@
       <c r="O208" s="223"/>
       <c r="P208" s="223"/>
     </row>
-    <row r="209" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="209" spans="1:19" ht="15" customHeight="1">
       <c r="A209" s="207" t="s">
         <v>1678</v>
       </c>
@@ -56751,7 +56756,7 @@
       <c r="O209" s="223"/>
       <c r="P209" s="223"/>
     </row>
-    <row r="210" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="210" spans="1:19" ht="15" customHeight="1">
       <c r="A210" s="207" t="s">
         <v>1679</v>
       </c>
@@ -56787,7 +56792,7 @@
       <c r="O210" s="223"/>
       <c r="P210" s="223"/>
     </row>
-    <row r="211" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="211" spans="1:19" ht="15" customHeight="1">
       <c r="A211" s="207" t="s">
         <v>1683</v>
       </c>
@@ -56821,7 +56826,7 @@
       <c r="O211" s="223"/>
       <c r="P211" s="223"/>
     </row>
-    <row r="212" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="212" spans="1:19" ht="15" customHeight="1">
       <c r="A212" s="203" t="s">
         <v>1690</v>
       </c>
@@ -56872,7 +56877,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="213" spans="1:19" ht="15" customHeight="1">
       <c r="A213" s="207" t="s">
         <v>1693</v>
       </c>
@@ -56906,7 +56911,7 @@
       <c r="O213" s="223"/>
       <c r="P213" s="223"/>
     </row>
-    <row r="214" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="214" spans="1:19" ht="15" customHeight="1">
       <c r="A214" s="207" t="s">
         <v>1697</v>
       </c>
@@ -56993,7 +56998,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="216" spans="1:19" ht="15" customHeight="1">
       <c r="A216" s="207" t="s">
         <v>1719</v>
       </c>
@@ -57091,9 +57096,7 @@
         <v>120</v>
       </c>
       <c r="D218" s="196"/>
-      <c r="E218" s="176" t="s">
-        <v>120</v>
-      </c>
+      <c r="E218" s="176"/>
       <c r="F218" s="177">
         <v>217</v>
       </c>
@@ -57124,7 +57127,7 @@
       </c>
       <c r="P218" s="223"/>
     </row>
-    <row r="219" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="219" spans="1:19" ht="15" customHeight="1">
       <c r="A219" s="207" t="s">
         <v>1736</v>
       </c>
@@ -57135,7 +57138,9 @@
         <v>120</v>
       </c>
       <c r="D219" s="196"/>
-      <c r="E219" s="196"/>
+      <c r="E219" s="176" t="s">
+        <v>120</v>
+      </c>
       <c r="F219" s="177">
         <v>218</v>
       </c>
@@ -57168,7 +57173,7 @@
       </c>
       <c r="P219" s="223"/>
     </row>
-    <row r="220" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="220" spans="1:19" ht="15" customHeight="1">
       <c r="A220" s="207" t="s">
         <v>1743</v>
       </c>
@@ -57208,7 +57213,7 @@
       <c r="O220" s="223"/>
       <c r="P220" s="223"/>
     </row>
-    <row r="221" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="221" spans="1:19" ht="15" customHeight="1">
       <c r="A221" s="207" t="s">
         <v>1750</v>
       </c>
@@ -57248,7 +57253,7 @@
       <c r="O221" s="223"/>
       <c r="P221" s="223"/>
     </row>
-    <row r="222" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="222" spans="1:19" ht="15" customHeight="1">
       <c r="A222" s="207" t="s">
         <v>1755</v>
       </c>
@@ -57288,7 +57293,7 @@
       <c r="O222" s="223"/>
       <c r="P222" s="223"/>
     </row>
-    <row r="223" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="223" spans="1:19" ht="15" customHeight="1">
       <c r="A223" s="207" t="s">
         <v>1759</v>
       </c>
@@ -57328,7 +57333,7 @@
       <c r="O223" s="223"/>
       <c r="P223" s="223"/>
     </row>
-    <row r="224" spans="1:19" ht="15" hidden="1" customHeight="1">
+    <row r="224" spans="1:19" ht="15" customHeight="1">
       <c r="A224" s="207" t="s">
         <v>1763</v>
       </c>
@@ -57368,7 +57373,7 @@
       <c r="O224" s="223"/>
       <c r="P224" s="223"/>
     </row>
-    <row r="225" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="225" spans="1:18" ht="15" customHeight="1">
       <c r="A225" s="207" t="s">
         <v>1765</v>
       </c>
@@ -57408,7 +57413,7 @@
       <c r="O225" s="223"/>
       <c r="P225" s="223"/>
     </row>
-    <row r="226" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="226" spans="1:18" ht="15" customHeight="1">
       <c r="A226" s="177" t="s">
         <v>1770</v>
       </c>
@@ -57460,7 +57465,7 @@
         <v>2875</v>
       </c>
     </row>
-    <row r="227" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="227" spans="1:18" ht="15" customHeight="1">
       <c r="A227" s="177" t="s">
         <v>1777</v>
       </c>
@@ -57514,7 +57519,7 @@
         <v>2875</v>
       </c>
     </row>
-    <row r="228" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="228" spans="1:18" ht="15" customHeight="1">
       <c r="A228" s="177" t="s">
         <v>1779</v>
       </c>
@@ -57608,7 +57613,7 @@
       <c r="O229" s="223"/>
       <c r="P229" s="223"/>
     </row>
-    <row r="230" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="230" spans="1:18" ht="15" customHeight="1">
       <c r="A230" s="207" t="s">
         <v>1875</v>
       </c>
@@ -57650,7 +57655,7 @@
       <c r="O230" s="223"/>
       <c r="P230" s="223"/>
     </row>
-    <row r="231" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="231" spans="1:18" ht="15" customHeight="1">
       <c r="A231" s="207" t="s">
         <v>1956</v>
       </c>
@@ -57690,7 +57695,7 @@
       <c r="O231" s="223"/>
       <c r="P231" s="223"/>
     </row>
-    <row r="232" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="232" spans="1:18" ht="15" customHeight="1">
       <c r="A232" s="207" t="s">
         <v>1958</v>
       </c>
@@ -57722,7 +57727,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="233" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="233" spans="1:18" ht="15" customHeight="1">
       <c r="A233" s="207" t="s">
         <v>1961</v>
       </c>
@@ -57754,7 +57759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="234" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="234" spans="1:18" ht="15" customHeight="1">
       <c r="A234" s="203" t="s">
         <v>2194</v>
       </c>
@@ -57788,7 +57793,7 @@
         <v>97.012365091844799</v>
       </c>
     </row>
-    <row r="235" spans="1:18" ht="15" hidden="1" customHeight="1">
+    <row r="235" spans="1:18" ht="15" customHeight="1">
       <c r="A235" s="223" t="s">
         <v>2606</v>
       </c>
@@ -57808,10 +57813,10 @@
       </c>
     </row>
     <row r="236" spans="1:18" ht="15" customHeight="1">
-      <c r="A236" s="237" t="s">
+      <c r="A236" s="236" t="s">
         <v>2880</v>
       </c>
-      <c r="C236" s="236" t="s">
+      <c r="C236" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E236" t="s">
@@ -57819,7 +57824,7 @@
       </c>
     </row>
     <row r="237" spans="1:18" ht="15" customHeight="1">
-      <c r="A237" s="237" t="s">
+      <c r="A237" s="236" t="s">
         <v>2881</v>
       </c>
       <c r="C237" s="232" t="s">
@@ -57836,10 +57841,10 @@
       </c>
     </row>
     <row r="238" spans="1:18" ht="15" customHeight="1">
-      <c r="A238" s="237" t="s">
+      <c r="A238" s="236" t="s">
         <v>2884</v>
       </c>
-      <c r="C238" s="236" t="s">
+      <c r="C238" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E238" t="s">
@@ -57847,7 +57852,7 @@
       </c>
     </row>
     <row r="239" spans="1:18" ht="15" customHeight="1">
-      <c r="A239" s="237" t="s">
+      <c r="A239" s="236" t="s">
         <v>2885</v>
       </c>
       <c r="C239" s="232" t="s">
@@ -57858,10 +57863,10 @@
       </c>
     </row>
     <row r="240" spans="1:18" ht="15" customHeight="1">
-      <c r="A240" s="237" t="s">
+      <c r="A240" s="236" t="s">
         <v>2887</v>
       </c>
-      <c r="C240" s="236" t="s">
+      <c r="C240" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E240" t="s">
@@ -57872,7 +57877,7 @@
       </c>
     </row>
     <row r="241" spans="1:12" ht="15" customHeight="1">
-      <c r="A241" s="237" t="s">
+      <c r="A241" s="236" t="s">
         <v>2888</v>
       </c>
       <c r="C241" s="232" t="s">
@@ -57886,10 +57891,10 @@
       </c>
     </row>
     <row r="242" spans="1:12" ht="15" customHeight="1">
-      <c r="A242" s="237" t="s">
+      <c r="A242" s="236" t="s">
         <v>2889</v>
       </c>
-      <c r="C242" s="236" t="s">
+      <c r="C242" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E242" t="s">
@@ -57900,7 +57905,7 @@
       </c>
     </row>
     <row r="243" spans="1:12" ht="15" customHeight="1">
-      <c r="A243" s="237" t="s">
+      <c r="A243" s="236" t="s">
         <v>2890</v>
       </c>
       <c r="C243" s="232" t="s">
@@ -57914,10 +57919,10 @@
       </c>
     </row>
     <row r="244" spans="1:12" ht="15" customHeight="1">
-      <c r="A244" s="237" t="s">
+      <c r="A244" s="236" t="s">
         <v>2823</v>
       </c>
-      <c r="C244" s="236" t="s">
+      <c r="C244" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E244" t="s">
@@ -57928,7 +57933,7 @@
       </c>
     </row>
     <row r="245" spans="1:12" ht="15" customHeight="1">
-      <c r="A245" s="237" t="s">
+      <c r="A245" s="236" t="s">
         <v>2891</v>
       </c>
       <c r="C245" s="232" t="s">
@@ -57942,10 +57947,10 @@
       </c>
     </row>
     <row r="246" spans="1:12" ht="15" customHeight="1">
-      <c r="A246" s="237" t="s">
+      <c r="A246" s="236" t="s">
         <v>2892</v>
       </c>
-      <c r="C246" s="236" t="s">
+      <c r="C246" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E246" t="s">
@@ -57956,10 +57961,10 @@
       </c>
     </row>
     <row r="247" spans="1:12" ht="15" customHeight="1">
-      <c r="A247" s="237" t="s">
+      <c r="A247" s="236" t="s">
         <v>2893</v>
       </c>
-      <c r="C247" s="236" t="s">
+      <c r="C247" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E247" t="s">
@@ -57973,7 +57978,7 @@
       <c r="A248" t="s">
         <v>2894</v>
       </c>
-      <c r="C248" s="236" t="s">
+      <c r="C248" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E248" t="s">
@@ -57984,10 +57989,10 @@
       </c>
     </row>
     <row r="249" spans="1:12" ht="15" customHeight="1">
-      <c r="A249" s="239" t="s">
+      <c r="A249" s="238" t="s">
         <v>2895</v>
       </c>
-      <c r="C249" s="236" t="s">
+      <c r="C249" s="232" t="s">
         <v>2879</v>
       </c>
       <c r="E249" t="s">
@@ -57997,14 +58002,19 @@
         <v>33.897942</v>
       </c>
     </row>
+    <row r="250" spans="1:12" ht="15" customHeight="1">
+      <c r="A250" s="239" t="s">
+        <v>2896</v>
+      </c>
+      <c r="C250" s="240" t="s">
+        <v>2879</v>
+      </c>
+      <c r="E250" s="223" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:S249" xr:uid="{B522DC56-3FF5-3344-845C-95A0430599ED}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S249" xr:uid="{B522DC56-3FF5-3344-845C-95A0430599ED}"/>
   <conditionalFormatting sqref="D2:G4 D5:E81 G5:G81 F5:F234">
     <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH(("Yes"),(D2))))</formula>

</xml_diff>

<commit_message>
Updated with missing plot
</commit_message>
<xml_diff>
--- a/1_Input_data/MasterCodebook_Final_June2022 ALL (Repaired).xlsx
+++ b/1_Input_data/MasterCodebook_Final_June2022 ALL (Repaired).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdamen/Documents/GitHub/Zika_imputation/1_Input_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmunozav/Desktop/Zika_imputation/1_Input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D93B330-25AB-D44F-B76D-D35E231B4AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33707836-293D-2D4A-BE9C-0A29955AC2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Var count and directions" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{EB9D8945-92F8-48A6-B1A8-0874D0F705AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{EB9D8945-92F8-48A6-B1A8-0874D0F705AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48005,10 +48005,10 @@
   <dimension ref="A1:T282"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E267" sqref="E267"/>
+      <selection pane="bottomRight" activeCell="Q283" sqref="Q283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>
@@ -49126,7 +49126,7 @@
       </c>
       <c r="O26" s="223"/>
       <c r="Q26" s="223" t="s">
-        <v>74</v>
+        <v>328</v>
       </c>
       <c r="S26">
         <v>1</v>
@@ -49170,7 +49170,7 @@
       </c>
       <c r="O27" s="223"/>
       <c r="Q27" s="223" t="s">
-        <v>74</v>
+        <v>328</v>
       </c>
       <c r="S27">
         <v>1</v>

</xml_diff>